<commit_message>
Alteração no banco de dados e forms e alterar dados
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -495,96 +491,60 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (27) 99978-7946</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>45782</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+          <t>(27)99978-7946</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>//</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>NÃO ATENDIDA</t>
+          <t>Não atendeu</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(27) 99727-7798</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>45782</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+          <t>(27)99727-7798</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
           <t>//</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>NÃO ATENDIDA</t>
+          <t>Não atendeu</t>
         </is>
       </c>
     </row>
@@ -596,21 +556,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>27 99576-8184</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>45772</v>
+          <t>(27)99576-8184</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>25/04/2025</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>Davi</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>11 anos</t>
-        </is>
+      <c r="E4" t="n">
+        <v>11</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -622,12 +582,14 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>45794</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>09:30:00</t>
+          <t>9:30</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -635,11 +597,7 @@
           <t>CTRL+TEENS</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>NÃO ATENDIDA</t>
-        </is>
-      </c>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -652,8 +610,10 @@
           <t>27 99742-7413</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>45782</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -675,12 +635,14 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="H5" s="2" t="n">
-        <v>45792</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>08:30:00</t>
+          <t>8:30</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -705,8 +667,10 @@
           <t>27 99747-0231</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>45782</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -728,11 +692,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
@@ -748,8 +708,10 @@
           <t>73 9960-2755</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>45782</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -771,11 +733,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -791,8 +749,10 @@
           <t>27 99699-5595</t>
         </is>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>45782</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -814,11 +774,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -834,8 +790,10 @@
           <t>27 99236-4455</t>
         </is>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>45782</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -857,11 +815,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -877,8 +831,10 @@
           <t>27 99854-3760</t>
         </is>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>45782</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -900,11 +856,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
@@ -920,8 +872,10 @@
           <t>27 99815-6749</t>
         </is>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>45782</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -943,11 +897,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
@@ -963,8 +913,10 @@
           <t>27 99916-7185</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>45782</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -986,11 +938,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
@@ -1006,8 +954,10 @@
           <t>27 99275-9660</t>
         </is>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>45782</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1029,11 +979,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -1049,8 +995,10 @@
           <t>27 99273-9041</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>45782</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1072,11 +1020,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
@@ -1092,8 +1036,10 @@
           <t>27 99657-3524</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>45782</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1115,11 +1061,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -1135,8 +1077,10 @@
           <t>27 99727-1902</t>
         </is>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>45782</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1158,11 +1102,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
@@ -1178,8 +1118,10 @@
           <t>28 99937-9193</t>
         </is>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>45782</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1201,11 +1143,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -1221,8 +1159,10 @@
           <t>27 99742-7926</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>45782</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1244,11 +1184,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -1264,8 +1200,10 @@
           <t>27 99707-2374</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>45782</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1287,11 +1225,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
@@ -1307,8 +1241,10 @@
           <t>27 99517-7812</t>
         </is>
       </c>
-      <c r="C20" s="2" t="n">
-        <v>45782</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1330,11 +1266,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -1350,8 +1282,10 @@
           <t>27 99783-7501</t>
         </is>
       </c>
-      <c r="C21" s="2" t="n">
-        <v>45782</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1373,11 +1307,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -1393,8 +1323,10 @@
           <t>27 99821-9252</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>45782</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1416,11 +1348,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
@@ -1436,8 +1364,10 @@
           <t>27 99913-6797</t>
         </is>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>45782</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1459,11 +1389,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
@@ -1479,8 +1405,10 @@
           <t>27 99840-2562</t>
         </is>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>45782</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1502,11 +1430,7 @@
           <t>Alta</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
@@ -1522,8 +1446,10 @@
           <t>27 99815-8960</t>
         </is>
       </c>
-      <c r="C25" s="2" t="n">
-        <v>45782</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1545,11 +1471,7 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
@@ -1565,8 +1487,10 @@
           <t>27 99977-8431</t>
         </is>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>45782</v>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1588,11 +1512,7 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
@@ -1608,8 +1528,10 @@
           <t>27 99890-9549</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>45782</v>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1631,11 +1553,7 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
@@ -1651,8 +1569,10 @@
           <t>27 99242-4361</t>
         </is>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>45782</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1674,11 +1594,7 @@
           <t>Pouco/Médio</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
@@ -1694,8 +1610,10 @@
           <t>27 99285-6406</t>
         </is>
       </c>
-      <c r="C29" s="2" t="n">
-        <v>45782</v>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1717,11 +1635,7 @@
           <t>Médio/Alta</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>tentando agendar</t>
-        </is>
-      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
@@ -1737,8 +1651,10 @@
           <t>27 99231-9428</t>
         </is>
       </c>
-      <c r="C30" s="2" t="n">
-        <v>45782</v>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1760,11 +1676,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
@@ -1780,8 +1692,10 @@
           <t>27 98846-3864</t>
         </is>
       </c>
-      <c r="C31" s="2" t="n">
-        <v>45783</v>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>06/05/2025</t>
+        </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1803,11 +1717,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
@@ -1823,8 +1733,10 @@
           <t>27 99863-1623</t>
         </is>
       </c>
-      <c r="C32" s="2" t="n">
-        <v>45783</v>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>06/05/2025</t>
+        </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1846,11 +1758,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
@@ -1866,8 +1774,10 @@
           <t>27 98865-7380</t>
         </is>
       </c>
-      <c r="C33" s="2" t="n">
-        <v>45783</v>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>06/05/2025</t>
+        </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1889,11 +1799,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
@@ -1909,8 +1815,10 @@
           <t>27 99231-5299</t>
         </is>
       </c>
-      <c r="C34" s="2" t="n">
-        <v>45776</v>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1932,11 +1840,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
@@ -1952,8 +1856,10 @@
           <t>27 98157-3763</t>
         </is>
       </c>
-      <c r="C35" s="2" t="n">
-        <v>45776</v>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1975,11 +1881,7 @@
           <t>Baixo</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
@@ -1995,8 +1897,10 @@
           <t>27 99756-5820</t>
         </is>
       </c>
-      <c r="C36" s="2" t="n">
-        <v>45784</v>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>07/05/2025</t>
+        </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -2018,11 +1922,7 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
@@ -2038,8 +1938,10 @@
           <t>27 98846-3864</t>
         </is>
       </c>
-      <c r="C37" s="2" t="n">
-        <v>45784</v>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>07/05/2025</t>
+        </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -2061,11 +1963,7 @@
           <t>Médio/Baixo</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
@@ -2081,8 +1979,10 @@
           <t>27 99746-2631</t>
         </is>
       </c>
-      <c r="C38" s="2" t="n">
-        <v>45784</v>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>07/05/2025</t>
+        </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -2104,11 +2004,7 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>tentando agendar</t>
-        </is>
-      </c>
+      <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
@@ -2124,8 +2020,10 @@
           <t>27 99810-5464</t>
         </is>
       </c>
-      <c r="C39" s="2" t="n">
-        <v>45769</v>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>22/04/2025</t>
+        </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -2147,16 +2045,8 @@
           <t>Alto</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Fechado</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>FECHADO</t>
-        </is>
-      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr">
         <is>
           <t>CTRL+TEENS</t>
@@ -2179,8 +2069,10 @@
           <t>28 99932-0801</t>
         </is>
       </c>
-      <c r="C40" s="2" t="n">
-        <v>45783</v>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>06/05/2025</t>
+        </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -2202,11 +2094,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
@@ -2222,8 +2110,10 @@
           <t>27 99668-7585</t>
         </is>
       </c>
-      <c r="C41" s="2" t="n">
-        <v>45783</v>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>06/05/2025</t>
+        </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -2245,11 +2135,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
@@ -2265,8 +2151,10 @@
           <t>27 99639-7085</t>
         </is>
       </c>
-      <c r="C42" s="2" t="n">
-        <v>45785</v>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>08/05/2025</t>
+        </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -2288,11 +2176,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
@@ -2308,8 +2192,10 @@
           <t>27 99958-5755</t>
         </is>
       </c>
-      <c r="C43" s="2" t="n">
-        <v>45785</v>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>08/05/2025</t>
+        </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -2331,11 +2217,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
@@ -2349,8 +2231,10 @@
       <c r="B44" t="n">
         <v>27999228225</v>
       </c>
-      <c r="C44" s="2" t="n">
-        <v>45786</v>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -2372,12 +2256,14 @@
           <t xml:space="preserve">Alta </t>
         </is>
       </c>
-      <c r="H44" s="2" t="n">
-        <v>45793</v>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>08:30:00</t>
+          <t>8:30</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -2402,8 +2288,10 @@
           <t>27 98893-4834</t>
         </is>
       </c>
-      <c r="C45" s="2" t="n">
-        <v>45786</v>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -2425,12 +2313,14 @@
           <t>Alta/Médio</t>
         </is>
       </c>
-      <c r="H45" s="2" t="n">
-        <v>45789</v>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>12/05/2025</t>
+        </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>08:30:00</t>
+          <t>8:30</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -2455,8 +2345,10 @@
           <t>27 99648-9024</t>
         </is>
       </c>
-      <c r="C46" s="2" t="n">
-        <v>45786</v>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -2478,11 +2370,7 @@
           <t>//</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr">
@@ -2502,8 +2390,10 @@
           <t>27 99648-0165</t>
         </is>
       </c>
-      <c r="C47" s="2" t="n">
-        <v>45789</v>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>12/05/2025</t>
+        </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -2525,11 +2415,7 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr">
@@ -2549,8 +2435,10 @@
           <t>27 99869-3274</t>
         </is>
       </c>
-      <c r="C48" s="2" t="n">
-        <v>45790</v>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -2572,12 +2460,14 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H48" s="2" t="n">
-        <v>45794</v>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>10:30:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -2602,8 +2492,10 @@
           <t>27 99686-7997</t>
         </is>
       </c>
-      <c r="C49" s="2" t="n">
-        <v>45791</v>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -2625,12 +2517,14 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H49" s="2" t="n">
-        <v>45792</v>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>08:30:00</t>
+          <t>8:30</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2653,8 +2547,10 @@
       <c r="B50" t="n">
         <v>27997612482</v>
       </c>
-      <c r="C50" s="2" t="n">
-        <v>45792</v>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -2676,12 +2572,14 @@
           <t>Médio</t>
         </is>
       </c>
-      <c r="H50" s="2" t="n">
-        <v>45794</v>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>10:30:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -2706,8 +2604,10 @@
           <t>27996408659</t>
         </is>
       </c>
-      <c r="C51" s="2" t="n">
-        <v>45790</v>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -2759,11 +2659,7 @@
           <t>dadad</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>dadas</t>
-        </is>
-      </c>
+      <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
           <t>Dasda</t>
@@ -2782,16 +2678,8 @@
           <t>Baixo</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>dadas</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>dasd</t>
-        </is>
-      </c>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr">
         <is>
           <t>sdada</t>
@@ -2814,11 +2702,7 @@
           <t>adada</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>dasda</t>
-        </is>
-      </c>
+      <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
           <t>Gada</t>
@@ -2837,16 +2721,8 @@
           <t>Baixo</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>dasds</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>dada</t>
-        </is>
-      </c>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr">
         <is>
           <t>CTRL+KIDS</t>
@@ -2899,7 +2775,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>08:30</t>
+          <t>8:30</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -2954,7 +2830,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>9:30</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">

</xml_diff>

<commit_message>
atualizacao banco de dados
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,16 @@
           <t>Ligação</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Lead</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo aluno</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -504,11 +514,7 @@
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -518,6 +524,16 @@
           <t>Não atendeu</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>ctrlplay</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -533,11 +549,7 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -547,6 +559,16 @@
           <t>Não atendeu</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>cna</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -597,7 +619,17 @@
           <t>CTRL+TEENS</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Não atendeu</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -607,7 +639,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>27 99742-7413</t>
+          <t>(27)99742-7413</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -620,21 +652,15 @@
           <t>Savio</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>10 anos</t>
-        </is>
+      <c r="E5" t="n">
+        <v>10</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>VESPERTINO</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>15/05/2025</t>
@@ -652,19 +678,21 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>ATENDIDA</t>
-        </is>
-      </c>
+          <t>Atendeu</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>27 99747-0231</t>
+          <t>(27)99747-0231</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -672,40 +700,32 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>10 anos</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Não atendeu</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>73 9960-2755</t>
+          <t>(73)9960-2755</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -715,38 +735,32 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Breno e Bernardo</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>12 e 7 (respectivamente)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+          <t>Breno E Bernardo</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>27 99699-5595</t>
+          <t>(27)99699-5595</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -754,40 +768,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>27 99236-4455</t>
+          <t>(27)99236-4455</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -795,40 +799,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>27 99854-3760</t>
+          <t>(27)99854-3760</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -836,40 +830,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>27 99815-6749</t>
+          <t>(27)99815-6749</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -877,40 +861,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>27 99916-7185</t>
+          <t>(27)99916-7185</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -918,40 +892,32 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>11 anos</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>27 99275-9660</t>
+          <t>(27)99275-9660</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -959,40 +925,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>27 99273-9041</t>
+          <t>(27)99273-9041</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1000,40 +956,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>27 99657-3524</t>
+          <t>(27)99657-3524</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1041,40 +987,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>27 99727-1902</t>
+          <t>(27)99727-1902</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1082,40 +1018,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>28 99937-9193</t>
+          <t>(28)99937-9193</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1123,40 +1049,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>27 99742-7926</t>
+          <t>(27)99742-7926</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1169,35 +1085,31 @@
           <t xml:space="preserve">Pedro </t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>7 anos</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="E18" t="n">
+        <v>7</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>27 99707-2374</t>
+          <t>(27)99707-2374</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1210,35 +1122,29 @@
           <t>Miguel</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>27 99517-7812</t>
+          <t>(27)99517-7812</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1246,40 +1152,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>27 99783-7501</t>
+          <t>(27)99783-7501</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1287,40 +1183,32 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>8 anos</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>27 99821-9252</t>
+          <t>(27)99821-9252</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1328,40 +1216,30 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr">
         <is>
-          <t>27 99913-6797</t>
+          <t>(27)99913-6797</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1369,40 +1247,36 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>13 anos</t>
-        </is>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>13</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>Quer ao mais profissional</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>27 99840-2562</t>
+          <t>(27)99840-2562</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1410,21 +1284,11 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>7 anos</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>7</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
           <t>Alta</t>
@@ -1433,7 +1297,17 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1443,7 +1317,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>27 99815-8960</t>
+          <t>(27)99815-8960</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1456,16 +1330,10 @@
           <t>Davi Lucas</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>11 anos</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="E25" t="n">
+        <v>11</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
           <t>Médio</t>
@@ -1474,7 +1342,17 @@
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1484,7 +1362,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>27 99977-8431</t>
+          <t>(27)99977-8431</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1497,10 +1375,8 @@
           <t>ROBERTH</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>9 anos</t>
-        </is>
+      <c r="E26" t="n">
+        <v>9</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1515,7 +1391,17 @@
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1525,7 +1411,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>27 99890-9549</t>
+          <t>(27)99890-9549</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1538,16 +1424,10 @@
           <t>Henzo Miguel</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>8 anos</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="E27" t="n">
+        <v>8</v>
+      </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
           <t>Médio</t>
@@ -1556,7 +1436,17 @@
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1566,7 +1456,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>27 99242-4361</t>
+          <t>(27)99242-4361</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1574,15 +1464,9 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>6 anos</t>
-        </is>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="n">
+        <v>6</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1597,7 +1481,17 @@
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1607,7 +1501,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>27 99285-6406</t>
+          <t>(27)99285-6406</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1620,10 +1514,8 @@
           <t>DÉRICK</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>7 anos em setembro</t>
-        </is>
+      <c r="E29" t="n">
+        <v>7</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1638,7 +1530,17 @@
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1648,7 +1550,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>27 99231-9428</t>
+          <t>(27)99231-9428</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1656,40 +1558,36 @@
           <t>05/05/2025</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>10 anos</t>
-        </is>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="n">
+        <v>10</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>faz 11 em outubro</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>27 98846-3864</t>
+          <t>(27)98846-3864</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1697,40 +1595,30 @@
           <t>06/05/2025</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>27 99863-1623</t>
+          <t>(27)99863-1623</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1738,40 +1626,30 @@
           <t>06/05/2025</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
-          <t>27 98865-7380</t>
+          <t>(27)98865-7380</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1779,30 +1657,24 @@
           <t>06/05/2025</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1812,7 +1684,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>27 99231-5299</t>
+          <t>(27)99231-5299</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1820,30 +1692,24 @@
           <t>29/04/2025</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1853,7 +1719,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>27 98157-3763</t>
+          <t>(27)98157-3763</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1866,16 +1732,10 @@
           <t>Lucas</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>10 anos</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="E35" t="n">
+        <v>10</v>
+      </c>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
           <t>Baixo</t>
@@ -1884,7 +1744,17 @@
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1894,7 +1764,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>27 99756-5820</t>
+          <t>(27)99756-5820</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1907,16 +1777,10 @@
           <t>Bernardo</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>8 anos</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="E36" t="n">
+        <v>8</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
           <t>Médio</t>
@@ -1925,7 +1789,17 @@
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1935,7 +1809,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>27 98846-3864</t>
+          <t>(27)98846-3864</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1948,10 +1822,8 @@
           <t>Geovana</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>17 anos</t>
-        </is>
+      <c r="E37" t="n">
+        <v>17</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1966,7 +1838,17 @@
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1976,7 +1858,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>27 99746-2631</t>
+          <t>(27)99746-2631</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1989,10 +1871,8 @@
           <t>Matheus</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>15 anos</t>
-        </is>
+      <c r="E38" t="n">
+        <v>15</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -2007,7 +1887,17 @@
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2017,7 +1907,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>27 99810-5464</t>
+          <t>(27)99810-5464</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2030,10 +1920,8 @@
           <t>Heittor Loriato Souza</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>14 anos</t>
-        </is>
+      <c r="E39" t="n">
+        <v>14</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -2054,19 +1942,21 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>ALUNO</t>
-        </is>
-      </c>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Indicação</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>28 99932-0801</t>
+          <t>(28)99932-0801</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2074,40 +1964,30 @@
           <t>06/05/2025</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>27 99668-7585</t>
+          <t>(27)99668-7585</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2115,30 +1995,28 @@
           <t>06/05/2025</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
-      <c r="K41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>cna</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2148,7 +2026,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>27 99639-7085</t>
+          <t>(27)99639-7085</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2156,30 +2034,26 @@
           <t>08/05/2025</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>7 anos</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="n">
+        <v>7</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2189,7 +2063,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>27 99958-5755</t>
+          <t>(27)99958-5755</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2197,30 +2071,24 @@
           <t>08/05/2025</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2228,8 +2096,10 @@
           <t>Tais</t>
         </is>
       </c>
-      <c r="B44" t="n">
-        <v>27999228225</v>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>(27)99922-8225</t>
+        </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -2241,21 +2111,15 @@
           <t>Lucas</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>8 anos</t>
-        </is>
+      <c r="E44" t="n">
+        <v>8</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
           <t>Gosta de jogos</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Alta </t>
-        </is>
-      </c>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
           <t>16/05/2025</t>
@@ -2273,9 +2137,15 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>ATENDIDA</t>
-        </is>
-      </c>
+          <t>Atendeu</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Indicação</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2285,7 +2155,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>27 98893-4834</t>
+          <t>(27)98893-4834</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2298,10 +2168,8 @@
           <t>Emily</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>11 anos</t>
-        </is>
+      <c r="E45" t="n">
+        <v>11</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2310,7 +2178,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Alta/Médio</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2330,19 +2198,21 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>NÃO ATENDIDA</t>
-        </is>
-      </c>
+          <t>Não atendeu</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
-          <t>27 99648-9024</t>
+          <t>(27)99648-9024</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2350,34 +2220,24 @@
           <t>09/05/2025</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>//</t>
-        </is>
-      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr">
         <is>
-          <t>NÃO ATENDIDA</t>
-        </is>
-      </c>
+          <t>Não atendeu</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2387,7 +2247,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>27 99648-0165</t>
+          <t>(27)99648-0165</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2400,14 +2260,12 @@
           <t>Nathan</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>10 anos</t>
-        </is>
+      <c r="E47" t="n">
+        <v>10</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> participou da colônia de férias da ctrl play </t>
+          <t>participou da colônia de férias da ctrl play</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2420,9 +2278,15 @@
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr">
         <is>
-          <t>NÃO ATENDIDA</t>
-        </is>
-      </c>
+          <t>Não atendeu</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2432,7 +2296,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>27 99869-3274</t>
+          <t>(27)99869-3274</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2445,10 +2309,8 @@
           <t>Valentina</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>8 anos</t>
-        </is>
+      <c r="E48" t="n">
+        <v>8</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2477,9 +2339,15 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>NÃO FEITA</t>
-        </is>
-      </c>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2489,7 +2357,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>27 99686-7997</t>
+          <t>(27)99686-7997</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2502,10 +2370,8 @@
           <t>Miguel</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>10 anos</t>
-        </is>
+      <c r="E49" t="n">
+        <v>10</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2534,9 +2400,15 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>NÃO FEITA</t>
-        </is>
-      </c>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2544,8 +2416,10 @@
           <t>Lorena</t>
         </is>
       </c>
-      <c r="B50" t="n">
-        <v>27997612482</v>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>(27)99761-2482</t>
+        </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2557,10 +2431,8 @@
           <t>Emanuel</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>9 anos</t>
-        </is>
+      <c r="E50" t="n">
+        <v>9</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2589,9 +2461,15 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>NÃO FEITA</t>
-        </is>
-      </c>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2601,7 +2479,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>27996408659</t>
+          <t>(27)99640-8659</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2644,119 +2522,131 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>NÃO FEITA</t>
-        </is>
-      </c>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Indicação</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Dasda</t>
+          <t>Gustavo</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>dadad</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr"/>
+          <t>(27)99711-0117</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Dasda</t>
+          <t>María Fernanda</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>dasdas</t>
+          <t>A filha tem natação na terça e pai folga as quartas</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Baixo</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>21/05/2025</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>08:30</t>
+        </is>
+      </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>sdada</t>
+          <t>CTRL+KIDS</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Feita</t>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>cna</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Dafa</t>
-        </is>
-      </c>
+      <c r="A53" t="inlineStr"/>
       <c r="B53" t="inlineStr">
         <is>
-          <t>adada</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Gada</t>
-        </is>
-      </c>
-      <c r="E53" t="n">
-        <v>21</v>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>dasda</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Baixo</t>
-        </is>
-      </c>
+          <t>(27)99821-2137</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>CTRL+KIDS</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>Feita</t>
-        </is>
-      </c>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Brendon</t>
+          <t>Livia</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>(27)99919-9096</t>
+          <t>(33)9180-5222</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16/05/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Carlos</t>
+          <t>Caio</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2765,57 +2655,55 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Médio</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>22/06/2025</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>8:30</t>
-        </is>
-      </c>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr">
         <is>
-          <t>CTRL+TEENS</t>
+          <t>CTRL+KIDS</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Não feita</t>
-        </is>
-      </c>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Dasd</t>
+          <t>Dirlei</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>(27)99919-9098</t>
+          <t>(27)99768-2508</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16/05/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Gfdf</t>
+          <t>Kevin</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>legal</t>
+          <t>Estuda no vespertino</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2825,35 +2713,41 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>20/12/2025</t>
+          <t>12/05/2025</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>9:30</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>CTRL+ADULTS</t>
+          <t>CTRL+TEENS</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Não atendida</t>
-        </is>
-      </c>
+          <t>Atendeu</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr">
         <is>
-          <t>(27)99919-9097</t>
+          <t>(27)99649-5426</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16/05/2025</t>
+          <t>10/05/2025</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
@@ -2864,31 +2758,588 @@
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Julia</t>
-        </is>
-      </c>
+      <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
-          <t>(27)99789-9410</t>
+          <t>(27)99975-9444</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16/05/2025</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Samuel</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>15</v>
+      </c>
       <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>(22)98844-0606</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>(27)98808-8756</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Sabrina</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>(27)99690-4455</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Sophia</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>13</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>MATUTINO</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>(27)98847-8393</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>(27)99816-5362</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>(27)99950-3328</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Valentina</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>7</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Irinna</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>(27)99720-0912</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Sara</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>13</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>MATUTINO até 12:30 - gosta de Robótica - Mãe mexe com Robótica</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>George</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>(27)98108-9823</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Kamily</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>12</v>
+      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>(27)99727-3529</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Alexandre</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>(27)99733-4010</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Ariana</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>(27)99958-0578</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Jayka</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>(27)99737-5889</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>José Luiz</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>11</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Michele</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>(27)99272-3756</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Lucas</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>10</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>MATUTINO</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>